<commit_message>
Fixed iPhone 4 screenshots - larger captions and more spacing.
</commit_message>
<xml_diff>
--- a/Documents/Promotional/Press Contacts/Contact Info.xlsx
+++ b/Documents/Promotional/Press Contacts/Contact Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="1940" windowWidth="36280" windowHeight="21380" tabRatio="500"/>
+    <workbookView xWindow="12560" yWindow="4460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="130">
   <si>
     <t>App Review Sites</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Followed Up?</t>
   </si>
   <si>
-    <t>Artists</t>
-  </si>
-  <si>
     <t>Sara Chen (Bayiu)</t>
   </si>
   <si>
@@ -397,6 +394,21 @@
   </si>
   <si>
     <t>Yes (18-Jul)</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Brian Chen</t>
+  </si>
+  <si>
+    <t>Joanna Stern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brianxchen@gmail.com  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">joanna.stern@wsj.com </t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -478,6 +490,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -536,7 +551,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -565,6 +580,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -900,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -938,7 +956,7 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -955,10 +973,10 @@
         <v>42187</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -975,10 +993,10 @@
         <v>42187</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -995,10 +1013,10 @@
         <v>42187</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1015,10 +1033,10 @@
         <v>42187</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1035,10 +1053,10 @@
         <v>42187</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1055,10 +1073,10 @@
         <v>42187</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1075,10 +1093,10 @@
         <v>42190</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1095,10 +1113,10 @@
         <v>42190</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1115,10 +1133,10 @@
         <v>42190</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1135,10 +1153,10 @@
         <v>42190</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1155,10 +1173,10 @@
         <v>42190</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1175,10 +1193,10 @@
         <v>42190</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1195,10 +1213,10 @@
         <v>42190</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1215,10 +1233,10 @@
         <v>42190</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1235,10 +1253,10 @@
         <v>42190</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1255,10 +1273,10 @@
         <v>42190</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1275,10 +1293,10 @@
         <v>42190</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1295,10 +1313,10 @@
         <v>42190</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1315,10 +1333,10 @@
         <v>42190</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1335,10 +1353,10 @@
         <v>42190</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1355,10 +1373,10 @@
         <v>42190</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1375,10 +1393,10 @@
         <v>42190</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1395,10 +1413,10 @@
         <v>42190</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1415,10 +1433,10 @@
         <v>42193</v>
       </c>
       <c r="E31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1435,26 +1453,50 @@
         <v>42193</v>
       </c>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="B34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="13"/>
+      <c r="A34" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="13"/>
+      <c r="A35" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
@@ -1480,7 +1522,7 @@
         <v>96</v>
       </c>
       <c r="F44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1502,10 +1544,10 @@
         <v>42187</v>
       </c>
       <c r="E46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1522,10 +1564,10 @@
         <v>42187</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1542,10 +1584,10 @@
         <v>42187</v>
       </c>
       <c r="E48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1556,16 +1598,16 @@
         <v>15249</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" s="7">
         <v>42188</v>
       </c>
       <c r="E50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1582,10 +1624,10 @@
         <v>42188</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1602,7 +1644,7 @@
         <v>42188</v>
       </c>
       <c r="F52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1619,10 +1661,10 @@
         <v>42188</v>
       </c>
       <c r="E53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1632,14 +1674,14 @@
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="2" t="s">
-        <v>117</v>
+      <c r="A55" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="B55" s="15">
-        <v>3030</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>120</v>
+        <v>183934</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="D55" s="7">
         <v>42203</v>
@@ -1649,50 +1691,50 @@
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="3" t="s">
-        <v>121</v>
+      <c r="A56" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B56" s="15">
-        <v>13878</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>122</v>
+        <v>3030</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="D56" s="7">
         <v>42203</v>
       </c>
       <c r="F56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="15">
-        <v>183934</v>
+        <v>13878</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D57" s="7">
         <v>42203</v>
       </c>
       <c r="F57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>16</v>
@@ -1704,59 +1746,59 @@
         <v>96</v>
       </c>
       <c r="F63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D65" s="7">
         <v>42200</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1794,12 +1836,15 @@
     <hyperlink ref="C51" r:id="rId31"/>
     <hyperlink ref="C65" r:id="rId32"/>
     <hyperlink ref="C71" r:id="rId33"/>
-    <hyperlink ref="C55" r:id="rId34"/>
-    <hyperlink ref="C56" r:id="rId35"/>
-    <hyperlink ref="C57" r:id="rId36"/>
+    <hyperlink ref="C56" r:id="rId34"/>
+    <hyperlink ref="C57" r:id="rId35"/>
+    <hyperlink ref="C55" r:id="rId36"/>
     <hyperlink ref="C50" r:id="rId37"/>
+    <hyperlink ref="C34" r:id="rId38"/>
+    <hyperlink ref="C35" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>